<commit_message>
SSDM-13256: Added missing columns for sample types.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-bare-sample-property.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-bare-sample-property.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t xml:space="preserve">SAMPLE_TYPE</t>
   </si>
@@ -40,6 +40,12 @@
     <t xml:space="preserve">Generated code prefix</t>
   </si>
   <si>
+    <t xml:space="preserve">Unique Subcodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">COURSE</t>
   </si>
   <si>
@@ -52,6 +58,12 @@
     <t xml:space="preserve">date_range_validation.py</t>
   </si>
   <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-11 17:23:44</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mandatory</t>
   </si>
   <si>
@@ -77,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">$NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
   </si>
   <si>
     <t xml:space="preserve">General info</t>
@@ -131,11 +140,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -174,6 +184,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -227,7 +245,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -252,6 +270,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -260,7 +286,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -268,7 +298,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,7 +322,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -327,177 +357,187 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="K2" s="0"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" s="3" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="8"/>
+      <c r="B5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="8"/>
+      <c r="E6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="8"/>
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="8"/>
+      <c r="A8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>33</v>
+      <c r="A9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>